<commit_message>
Refactoring on style and size copying.
</commit_message>
<xml_diff>
--- a/examples/docs-output.xlsx
+++ b/examples/docs-output.xlsx
@@ -1507,7 +1507,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="9" customWidth="1"/>
     <col min="7" max="256" width="16.3516" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1734,7 +1739,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="10" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="10" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="10" customWidth="1"/>
+    <col min="3" max="6" width="16.3516" style="10" customWidth="1"/>
     <col min="7" max="256" width="16.3516" style="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1761,7 +1768,7 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="6">
         <v>12</v>
       </c>
@@ -1771,7 +1778,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="6">
         <v>13</v>
       </c>
@@ -1781,7 +1788,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="6">
         <v>14</v>
       </c>
@@ -1791,7 +1798,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="6">
         <v>15</v>
       </c>
@@ -1813,7 +1820,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="6">
         <v>22</v>
       </c>
@@ -1823,7 +1830,7 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="6">
         <v>23</v>
       </c>
@@ -1833,7 +1840,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="8"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="6">
         <v>24</v>
       </c>
@@ -1843,7 +1850,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="8"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="6">
         <v>25</v>
       </c>
@@ -1865,7 +1872,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="8"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="6">
         <v>32</v>
       </c>
@@ -1875,7 +1882,7 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="8"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="6">
         <v>33</v>
       </c>
@@ -1885,7 +1892,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="6">
         <v>34</v>
       </c>
@@ -1895,7 +1902,7 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="6">
         <v>35</v>
       </c>

</xml_diff>